<commit_message>
Update MASTER Education Classes Roster.xlsx
</commit_message>
<xml_diff>
--- a/training/upload/MASTER Education Classes Roster.xlsx
+++ b/training/upload/MASTER Education Classes Roster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronbell/Desktop/CrewOps360/training/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6460FCC7-0137-42AA-AC61-58A9E9C999DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67C88C12-CA33-4042-8E58-9248710F7659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="17240" firstSheet="3" activeTab="12" xr2:uid="{5604E27C-0991-9B4E-A9D1-5F87A876A78F}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="17240" firstSheet="3" xr2:uid="{5604E27C-0991-9B4E-A9D1-5F87A876A78F}"/>
   </bookViews>
   <sheets>
     <sheet name="Class_Enrollment" sheetId="1" r:id="rId1"/>
@@ -1537,9 +1537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE3E758-B252-634C-B9B3-AE34AE7DE6C7}">
   <dimension ref="A1:P155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E138" sqref="E138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="E34" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P40" sqref="P40"/>
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3560,7 +3560,7 @@
         <v>1</v>
       </c>
       <c r="P40" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -4310,7 +4310,7 @@
         <v>1</v>
       </c>
       <c r="P55" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -5010,7 +5010,7 @@
         <v>1</v>
       </c>
       <c r="P69" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:16">
@@ -5610,7 +5610,7 @@
         <v>0</v>
       </c>
       <c r="P81" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:16">
@@ -5660,7 +5660,7 @@
         <v>1</v>
       </c>
       <c r="P82" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:16">
@@ -9200,7 +9200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0587D0-89DF-4D05-A902-12BFC82DD3EC}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>